<commit_message>
Added all functionality without sending emails
</commit_message>
<xml_diff>
--- a/InvoiceSenderControl.xlsx
+++ b/InvoiceSenderControl.xlsx
@@ -73,7 +73,7 @@
     <t>Dear Ms Smith,</t>
   </si>
   <si>
-    <t>Maria Nowak</t>
+    <t>Mikołaj Męderski</t>
   </si>
   <si>
     <t>nowak@gmail.com</t>
@@ -92,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -112,6 +112,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -138,6 +139,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -444,7 +448,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">

</xml_diff>

<commit_message>
Added email subject and message Id to excel with SMTP information
</commit_message>
<xml_diff>
--- a/InvoiceSenderControl.xlsx
+++ b/InvoiceSenderControl.xlsx
@@ -11,24 +11,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Note: Put your invoices in "invoices" directory</t>
   </si>
   <si>
-    <t>Then execute python script (double click on execute.py). Note: python 3.0 must be installed!</t>
-  </si>
-  <si>
-    <t>In example below, every invoce with "ExampleCompanyName" text will be sent to office@microsoft.com.</t>
+    <t>Then execute python script (double click on execute.py).
+Note: python 3.0 must be installed!</t>
+  </si>
+  <si>
+    <t>SMTP address:</t>
+  </si>
+  <si>
+    <t>SMTP port:</t>
+  </si>
+  <si>
+    <t>Source email address:</t>
+  </si>
+  <si>
+    <t>Password / App Password:
+For security reasons leave empty
+(will be prompt for it during script execution)</t>
+  </si>
+  <si>
+    <t>About App  Password:
+https://support.google.com/accounts/answer/185833</t>
+  </si>
+  <si>
+    <t>In example below, every invoce with
+"ExampleCompanyName" text
+will be sent to office@microsoft.com.</t>
   </si>
   <si>
     <t>To get python see: https://www.python.org/downloads/</t>
   </si>
   <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>587</t>
+  </si>
+  <si>
+    <t>youremail@gmail.com</t>
+  </si>
+  <si>
     <t>Words to use in email template (you can add more):</t>
   </si>
   <si>
-    <t>Here add text, which should be found in invoice (company name or person name/surname)</t>
+    <t>Here add text, which should be found in invoice
+(company name or person name/surname)</t>
   </si>
   <si>
     <t>Here write target email</t>
@@ -37,6 +68,13 @@
     <t>Template file name</t>
   </si>
   <si>
+    <t>Email Subject</t>
+  </si>
+  <si>
+    <t>MessageID (Leave empty 
+if don't want to continue thread)</t>
+  </si>
+  <si>
     <t>[TITLE]</t>
   </si>
   <si>
@@ -55,6 +93,9 @@
     <t>EmailTemplateEng.txt</t>
   </si>
   <si>
+    <t>Payments for appartment</t>
+  </si>
+  <si>
     <t>Dear Sir/Madam,</t>
   </si>
   <si>
@@ -70,16 +111,22 @@
     <t>catherine@gmail.com</t>
   </si>
   <si>
+    <t>Your invoices</t>
+  </si>
+  <si>
     <t>Dear Ms Smith,</t>
   </si>
   <si>
-    <t>Mikołaj Męderski</t>
+    <t>Maria Nowak</t>
   </si>
   <si>
     <t>nowak@gmail.com</t>
   </si>
   <si>
     <t>EmailTemplatePol.txt</t>
+  </si>
+  <si>
+    <t>Faktury za mieszkanie</t>
   </si>
   <si>
     <t>Szanowna Pani Mario,</t>
@@ -92,7 +139,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -105,8 +152,22 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFF0000"/>
+    </font>
+    <font>
+      <color rgb="FFFF0000"/>
     </font>
     <font>
       <color theme="1"/>
@@ -128,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -142,6 +203,19 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -361,11 +435,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="4.57"/>
-    <col customWidth="1" min="2" max="2" width="94.43"/>
-    <col customWidth="1" min="3" max="3" width="83.29"/>
+    <col customWidth="1" min="2" max="2" width="45.86"/>
+    <col customWidth="1" min="3" max="3" width="53.29"/>
     <col customWidth="1" min="4" max="4" width="29.57"/>
-    <col customWidth="1" min="5" max="5" width="31.86"/>
-    <col customWidth="1" min="7" max="7" width="31.43"/>
+    <col customWidth="1" min="5" max="5" width="28.14"/>
+    <col customWidth="1" min="6" max="7" width="31.86"/>
+    <col customWidth="1" min="8" max="8" width="25.29"/>
+    <col customWidth="1" min="9" max="9" width="16.43"/>
+    <col customWidth="1" min="10" max="10" width="23.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -375,99 +452,145 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" ht="44.25" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" ht="36.0" customHeight="1">
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="H5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>16</v>
+      <c r="B6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="H6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>16</v>
+      <c r="B7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="H7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>